<commit_message>
Code for change for Meter Stuck, Burnt, Replace. To be tested.
</commit_message>
<xml_diff>
--- a/Docs/Testing/Stuck & Burnt cases.xlsx
+++ b/Docs/Testing/Stuck & Burnt cases.xlsx
@@ -50,6 +50,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>st</t>
     </r>
@@ -58,6 +59,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t> Jan</t>
     </r>
@@ -72,6 +74,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>th</t>
     </r>
@@ -80,6 +83,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t> Jan</t>
     </r>
@@ -106,6 +110,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>th</t>
     </r>
@@ -114,6 +119,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t> Jan</t>
     </r>
@@ -149,6 +155,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,20 +177,28 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,8 +244,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -250,10 +273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -263,274 +286,421 @@
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="K2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="0"/>
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="0"/>
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="0"/>
+      <c r="F10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C12" s="1" t="n">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C14" s="1" t="n">
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C14" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="0"/>
+      <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C16" s="1" t="n">
+      <c r="K14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="0"/>
+      <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C18" s="1" t="n">
+      <c r="K16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="0"/>
+      <c r="F18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="K18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C20" s="1" t="n">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>